<commit_message>
warning messages ignored in ploting
</commit_message>
<xml_diff>
--- a/config/long_variable_names_to_short_variable_names.xlsx
+++ b/config/long_variable_names_to_short_variable_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\power-model\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\finn_dev_branch\power-model\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F484437E-97B8-4E7F-9377-E97918A3A2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D848EC-97F1-469B-A87C-8FD98FC55DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27045" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="25905" windowHeight="14655" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMISSION" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="286">
   <si>
     <t>1_xC02</t>
   </si>
@@ -879,6 +879,9 @@
   </si>
   <si>
     <t>08_01_natural_gas_CCS_CO2</t>
+  </si>
+  <si>
+    <t>17Dx</t>
   </si>
 </sst>
 </file>
@@ -1248,12 +1251,12 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>185</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>278</v>
       </c>
@@ -1269,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>279</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>280</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>281</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>282</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>283</v>
       </c>
@@ -1309,7 +1312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>284</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1325,7 +1328,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1346,9 +1349,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>185</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1364,7 +1367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1372,7 +1375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1388,7 +1391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1412,7 +1415,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1428,7 +1431,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1444,7 +1447,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1452,7 +1455,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1484,7 +1487,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -1508,7 +1511,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -1524,7 +1527,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -1580,7 +1583,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>69</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -1612,7 +1615,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
@@ -1620,7 +1623,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>79</v>
       </c>
@@ -1636,7 +1639,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -1653,16 +1656,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>185</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -1678,15 +1681,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
@@ -1694,7 +1697,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>89</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>229</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>230</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>231</v>
       </c>
@@ -1734,7 +1737,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>233</v>
       </c>
@@ -1750,7 +1753,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>234</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>235</v>
       </c>
@@ -1766,7 +1769,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>236</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>237</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>100</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>102</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>238</v>
       </c>
@@ -1806,7 +1809,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>105</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>107</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>109</v>
       </c>
@@ -1839,17 +1842,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.453125" customWidth="1"/>
-    <col min="4" max="4" width="46.7265625" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>185</v>
       </c>
@@ -1857,7 +1860,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
@@ -1865,7 +1868,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>240</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>241</v>
       </c>
@@ -1881,7 +1884,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>242</v>
       </c>
@@ -1889,7 +1892,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>113</v>
       </c>
@@ -1897,7 +1900,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1905,7 +1908,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>243</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>244</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>117</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>119</v>
       </c>
@@ -1937,7 +1940,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>121</v>
       </c>
@@ -1945,7 +1948,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>245</v>
       </c>
@@ -1953,7 +1956,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>246</v>
       </c>
@@ -1961,7 +1964,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>123</v>
       </c>
@@ -1969,7 +1972,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>125</v>
       </c>
@@ -1977,7 +1980,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>127</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>129</v>
       </c>
@@ -1993,7 +1996,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>247</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>248</v>
       </c>
@@ -2009,7 +2012,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>131</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>133</v>
       </c>
@@ -2025,7 +2028,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>249</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>250</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>251</v>
       </c>
@@ -2049,7 +2052,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>252</v>
       </c>
@@ -2057,7 +2060,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>253</v>
       </c>
@@ -2065,7 +2068,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>254</v>
       </c>
@@ -2073,7 +2076,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>255</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>256</v>
       </c>
@@ -2089,7 +2092,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>142</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>144</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>146</v>
       </c>
@@ -2113,7 +2116,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>148</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>150</v>
       </c>
@@ -2129,7 +2132,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>152</v>
       </c>
@@ -2137,7 +2140,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>154</v>
       </c>
@@ -2145,7 +2148,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>257</v>
       </c>
@@ -2153,7 +2156,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>258</v>
       </c>
@@ -2161,7 +2164,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>259</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>260</v>
       </c>
@@ -2177,7 +2180,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>261</v>
       </c>
@@ -2185,7 +2188,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>262</v>
       </c>
@@ -2193,7 +2196,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>263</v>
       </c>
@@ -2201,7 +2204,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>163</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>165</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>167</v>
       </c>
@@ -2225,7 +2228,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>169</v>
       </c>
@@ -2233,7 +2236,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>171</v>
       </c>
@@ -2241,7 +2244,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>173</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>175</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>264</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>265</v>
       </c>
@@ -2273,7 +2276,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>177</v>
       </c>
@@ -2281,7 +2284,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>179</v>
       </c>
@@ -2289,7 +2292,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>181</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>183</v>
       </c>
@@ -2318,9 +2321,9 @@
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>185</v>
       </c>
@@ -2328,7 +2331,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>187</v>
       </c>
@@ -2336,7 +2339,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -2344,7 +2347,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>191</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>193</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -2368,7 +2371,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -2376,7 +2379,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>201</v>
       </c>
@@ -2392,7 +2395,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>203</v>
       </c>
@@ -2400,7 +2403,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>205</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>209</v>
       </c>
@@ -2424,7 +2427,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>211</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>213</v>
       </c>
@@ -2440,7 +2443,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>215</v>
       </c>
@@ -2448,7 +2451,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>217</v>
       </c>
@@ -2456,7 +2459,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>219</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>221</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>223</v>
       </c>
@@ -2480,7 +2483,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>225</v>
       </c>
@@ -2488,7 +2491,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>227</v>
       </c>

</xml_diff>